<commit_message>
validando importador de solicitudes
</commit_message>
<xml_diff>
--- a/ComprasCartonesLGP.Web/Areas/Data/Uploads/SOLICITUDES DIGITALES 551.xlsx
+++ b/ComprasCartonesLGP.Web/Areas/Data/Uploads/SOLICITUDES DIGITALES 551.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\COPIA MARIELA 11-06-2020\PROMOCION 2021\STARNET PLATAFORMA DIGITAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isidro\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="551 sol.digitales" sheetId="1" r:id="rId1"/>
@@ -58,10 +58,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -354,7 +354,7 @@
   <dimension ref="A1:A553"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -373,9 +373,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>49</v>
-      </c>
+      <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">

</xml_diff>